<commit_message>
Vanilla Persona Weapons Expanded 수정
</commit_message>
<xml_diff>
--- a/Data/Vanilla Expanded/Vanilla Persona Weapons Expanded - 2826922787/2826922787.xlsx
+++ b/Data/Vanilla Expanded/Vanilla Persona Weapons Expanded - 2826922787/2826922787.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\RimWorld\Mods\RMK\Data\Vanilla Expanded\Vanilla Persona Weapons Expanded - 2826922787\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC897AC0-9C0E-4F8F-B5D1-EECC21BD8A11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A1ACD91-8E45-4467-B5C5-726593512959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Main_240306" sheetId="3" r:id="rId1"/>
+    <sheet name="Main_240307" sheetId="3" r:id="rId1"/>
     <sheet name="240128" sheetId="1" r:id="rId2"/>
     <sheet name="Merge" sheetId="2" r:id="rId3"/>
   </sheets>

</xml_diff>